<commit_message>
finish B1 & B2
</commit_message>
<xml_diff>
--- a/gouzhiyuan/evidence.xlsx
+++ b/gouzhiyuan/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gouzhiyuan/workspace/GitHub/gon-evidence/gouzhiyuan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD4C706-3AD2-3A4B-BDFA-1EA9F6DD8AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF08203-E5C2-7647-94F8-8C3F8B2287CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5660" yWindow="760" windowWidth="28900" windowHeight="21580" tabRatio="500" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5660" yWindow="760" windowWidth="28900" windowHeight="21580" tabRatio="500" firstSheet="7" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="89">
   <si>
     <t>TeamName</t>
   </si>
@@ -315,6 +315,18 @@
   </si>
   <si>
     <t>r36</t>
+  </si>
+  <si>
+    <t>FB17469645ACDBDA2CD7C7EF27063C1DFA88C4CE0CFBECB231D49F4E4FBB6A33</t>
+  </si>
+  <si>
+    <t>92945CAA5FAE911EA7270912CDA3CBC3412FB4481318324EB7162B8D7BB86DF9</t>
+  </si>
+  <si>
+    <t>F901B7318DD925DA53168062BB795E6A306BCB2B26327BCF55987998A67DF384</t>
+  </si>
+  <si>
+    <t>0D7643BA695D83810B41A4AC279119FE67822A8DB6203B2C6DB7998B3E0DA1A6</t>
   </si>
 </sst>
 </file>
@@ -927,7 +939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1503,7 +1515,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P49" sqref="P49"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <sheetData>
@@ -1514,12 +1528,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.5" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1537,8 +1551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -1550,12 +1564,12 @@
     </row>
     <row r="2" spans="1:1" ht="14">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>